<commit_message>
Fix CTDC static data
</commit_message>
<xml_diff>
--- a/InputFiles/CTDC/CTDC_StaticData.xlsx
+++ b/InputFiles/CTDC/CTDC_StaticData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leungvw/git/Commons_Automation/InputFiles/CTDC/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leungvw/git2/Commons_Automation/InputFiles/CTDC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D675FC7-26E9-7046-A971-751EA19F048B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2602B6B3-FDAB-CE4C-8225-27F10E47EDBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3560" yWindow="1820" windowWidth="31040" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3560" yWindow="1820" windowWidth="31040" windowHeight="20120" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="V_HomePage" sheetId="1" r:id="rId1"/>
@@ -550,7 +550,7 @@
   </si>
   <si>
     <t>The Clinical and Translational Data Commons (CTDC) is designed to facilitate the integration and analysis of a wide array of clinical and translational research data. To support this initiative, the CTDC will accept a variety of data types, each crucial for the comprehensive understanding of clinical outcomes and the translational pathway from laboratory and clinical research to clinical applications.
-Those interested in submitting data to the CTDC must first fill out a data submission request through the CRDC Submission Portal. Requests will be reviewed to assess alignment with CTDC and CRDC’s mission and overall data requirements. Review times can be expected to be four to six weeks. For more information regarding submission requests and data submission, see CRDC’s Submit Data page.
+Those interested in submitting data to the CTDC must first fill out a data submission request through the CRDC Submission Portal. Requests will be reviewed to assess alignment with CTDC and CRDC’s mission and overall data requirements. Review times can be expected to be four to six weeks. For more information regarding submission requests and data submission, see CRDC’s Submit Data page or contact NCICRDC@mail.nih.gov✉️.
 Below are the primary categories of data the CTDC currently accepts:
 De-identified Clinical Data:
 Patient demographics
@@ -602,7 +602,8 @@
   <si>
     <t>GraphQL is a powerful query language for APIs. It provides a more efficient, powerful, and flexible alternative to the traditional REST API. Unlike traditional REST APIs, which typically require multiple endpoints to retrieve various pieces of data, GraphQL allows clients (the systems making the queries) to fetch exactly what they need in a single request. The Clinical and Translational Data Commons (CTDC) leverages this technology by offering a GraphQL API interface, which enables users to interact with CTDC data directly from their own systems, such as through Jupyter notebooks.
 To begin querying the CTDC data via GraphQL, access our API endpoint at https://clinical-qa.datacommons.cancer.gov/v1/graphql/.
-If you are new to GraphQL and want to learn more about query language, comprehensive tutorials and example queries are available at graphql.org. These resources provide an excellent starting point for understanding and utilizing GraphQL effectively.</t>
+If you are new to GraphQL and want to learn more about query language, comprehensive tutorials and example queries are available at graphql.org. These resources provide an excellent starting point for understanding and utilizing GraphQL effectively.
+Below is the GraphiQL integrated development environment (IDE), from here you can query the data within the Clinical and Translational Data Commons database. The default query below is the same query that is used to query data from the Clinical and Translational Data Commons database for the Global Stats Bar.</t>
   </si>
 </sst>
 </file>
@@ -936,7 +937,7 @@
   </sheetPr>
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+    <sheetView zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
@@ -1739,7 +1740,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1813,8 +1814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D035CF3-778E-2D43-8BD7-090C74996720}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1843,7 +1844,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="182" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" ht="238" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>93</v>
       </c>

</xml_diff>

<commit_message>
Add PBAC positive and negative scenarios
</commit_message>
<xml_diff>
--- a/InputFiles/CTDC/CTDC_StaticData.xlsx
+++ b/InputFiles/CTDC/CTDC_StaticData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leungvw/git2/Commons_Automation/InputFiles/CTDC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2602B6B3-FDAB-CE4C-8225-27F10E47EDBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FADC7135-538C-F045-B1A9-84490C0F6F51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3560" yWindow="1820" windowWidth="31040" windowHeight="20120" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3560" yWindow="1820" windowWidth="31040" windowHeight="20120" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="V_HomePage" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="160">
   <si>
     <t>verificationText</t>
   </si>
@@ -324,12 +324,6 @@
     <t>GraphQLDescription</t>
   </si>
   <si>
-    <t>https://clinical-qa.datacommons.cancer.gov/v1/graphql/</t>
-  </si>
-  <si>
-    <t>ApiLink</t>
-  </si>
-  <si>
     <t>https://graphql.org/learn/</t>
   </si>
   <si>
@@ -404,9 +398,6 @@
   </si>
   <si>
     <t>Support</t>
-  </si>
-  <si>
-    <t>If you have any questions, please contact us at NCICTDCHelpDesk@mail.nih.gov.</t>
   </si>
   <si>
     <t>ContactDescription</t>
@@ -604,6 +595,15 @@
 To begin querying the CTDC data via GraphQL, access our API endpoint at https://clinical-qa.datacommons.cancer.gov/v1/graphql/.
 If you are new to GraphQL and want to learn more about query language, comprehensive tutorials and example queries are available at graphql.org. These resources provide an excellent starting point for understanding and utilizing GraphQL effectively.
 Below is the GraphiQL integrated development environment (IDE), from here you can query the data within the Clinical and Translational Data Commons database. The default query below is the same query that is used to query data from the Clinical and Translational Data Commons database for the Global Stats Bar.</t>
+  </si>
+  <si>
+    <t>mailto:type: email NCICRDC@mail.nih.gov</t>
+  </si>
+  <si>
+    <t>If you have any questions, please contact us at NCICRDC@mail.nih.gov✉️.</t>
+  </si>
+  <si>
+    <t>NCICRDC@mail.nih.gov✉️</t>
   </si>
 </sst>
 </file>
@@ -988,7 +988,7 @@
         <v>26</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="14" x14ac:dyDescent="0.15">
@@ -1119,7 +1119,7 @@
     </row>
     <row r="19" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>51</v>
@@ -1159,8 +1159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C402EDB-B8AB-444E-A99A-64CDE22BCAB7}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1186,31 +1186,31 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>117</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="B4" s="14" t="s">
-        <v>82</v>
+      <c r="B4" s="10" t="s">
+        <v>159</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>83</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1" xr:uid="{1C6EDCFE-751E-B34C-BB4A-204084CDC452}"/>
+    <hyperlink ref="C4" r:id="rId1" display="mailto:NCICTDCHelpDesk@mail.nih.gov" xr:uid="{1C6EDCFE-751E-B34C-BB4A-204084CDC452}"/>
     <hyperlink ref="B4" r:id="rId2" xr:uid="{CC523369-A760-F542-92AE-ECECCCFF0F0C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1253,130 +1253,130 @@
     </row>
     <row r="3" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="42" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="56" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="140" x14ac:dyDescent="0.15">
       <c r="A7" s="7" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="7" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="7" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="7" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" s="7" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="7" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" s="7" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -1448,7 +1448,7 @@
         <v>55</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="14" x14ac:dyDescent="0.15">
@@ -1519,7 +1519,7 @@
         <v>59</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>60</v>
@@ -1673,7 +1673,7 @@
         <v>75</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
@@ -1774,7 +1774,7 @@
         <v>86</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
@@ -1812,10 +1812,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D035CF3-778E-2D43-8BD7-090C74996720}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1849,37 +1849,24 @@
         <v>93</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="14" t="s">
         <v>95</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>94</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A5" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>96</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1" xr:uid="{6D827E7E-F057-3B41-A62A-FE3281E9DA0D}"/>
-    <hyperlink ref="B5" r:id="rId2" display="https://github.com/CBIIT/ctdc-model" xr:uid="{9CBB4150-93A0-094D-B436-BC6AF4AAE26F}"/>
-    <hyperlink ref="C5" r:id="rId3" xr:uid="{D04D7E84-1F13-1045-919A-38E965FCAFE9}"/>
-    <hyperlink ref="B4" r:id="rId4" xr:uid="{069D5F14-889E-9F4B-8574-0B8184207ECF}"/>
+    <hyperlink ref="B4" r:id="rId1" display="https://github.com/CBIIT/ctdc-model" xr:uid="{9CBB4150-93A0-094D-B436-BC6AF4AAE26F}"/>
+    <hyperlink ref="C4" r:id="rId2" xr:uid="{D04D7E84-1F13-1045-919A-38E965FCAFE9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1916,34 +1903,34 @@
         <v>6</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="238" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>101</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>60</v>
@@ -1991,23 +1978,23 @@
         <v>6</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="357" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>15</v>
@@ -2018,21 +2005,21 @@
         <v>21</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="C6" t="s">
         <v>112</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="C6" t="s">
-        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>